<commit_message>
Updated folder with new files
</commit_message>
<xml_diff>
--- a/admin/output/schedule_report.xlsx
+++ b/admin/output/schedule_report.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Floor 1" sheetId="1" r:id="rId4"/>
     <sheet name="Floor 2" sheetId="2" r:id="rId5"/>
-    <sheet name="Floor 3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
   <si>
     <t>Floor: 1</t>
   </si>
@@ -46,34 +45,28 @@
     <t>End Time</t>
   </si>
   <si>
-    <t>ITE 314</t>
+    <t>ITC 131</t>
+  </si>
+  <si>
+    <t>Francis  Rivas</t>
+  </si>
+  <si>
+    <t>07:00:00</t>
+  </si>
+  <si>
+    <t>08:30:00</t>
+  </si>
+  <si>
+    <t>Floor: 2</t>
+  </si>
+  <si>
+    <t>Room: 201</t>
+  </si>
+  <si>
+    <t>ITC</t>
   </si>
   <si>
     <t>John  Doe</t>
-  </si>
-  <si>
-    <t>07:00:00</t>
-  </si>
-  <si>
-    <t>08:30:00</t>
-  </si>
-  <si>
-    <t>ITC 314</t>
-  </si>
-  <si>
-    <t>Francis  Rivas</t>
-  </si>
-  <si>
-    <t>Floor: 2</t>
-  </si>
-  <si>
-    <t>Room: 201</t>
-  </si>
-  <si>
-    <t>Floor: 3</t>
-  </si>
-  <si>
-    <t>Room: 301</t>
   </si>
 </sst>
 </file>
@@ -419,7 +412,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="I6" sqref="I6:L6"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -503,18 +496,6 @@
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -539,115 +520,6 @@
   </sheetPr>
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A6" sqref="A6:D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:H4"/>
-    <mergeCell ref="I4:L4"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:L6"/>
-  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
@@ -656,12 +528,12 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -724,10 +596,10 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>

</xml_diff>